<commit_message>
idk its the update
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -13,15 +13,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">bookshelf - unmovable</t>
   </si>
   <si>
+    <t xml:space="preserve">empty - has batteries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empty - has bug</t>
+  </si>
+  <si>
     <t xml:space="preserve">desk - has printer - movable</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0 - start - has flashdrive</t>
+    <t xml:space="preserve">empty - has paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0 - start - has flashdrive and lamp</t>
   </si>
   <si>
     <t xml:space="preserve">desk - unmovable</t>
@@ -36,9 +45,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -607,20 +616,24 @@
     <row r="1" ht="56.25" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" ht="67.5" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -630,41 +643,43 @@
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="71.25" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" ht="70.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>